<commit_message>
Drive testcases through Excel
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,71 +1,87 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayur_sapre\eclipse-workspace\SeleniumAutomation\src\test\resources\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912363E8-0BF3-4283-9514-2C5BC0890F57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{03E8BCAA-FF3E-473E-86C9-12A12C811D3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D5E31465-B114-4177-9652-2EC0C5400E2C}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15465" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
+    <sheet name="DATA" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:I14"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
+  <si>
+    <t>testdescription</t>
+  </si>
+  <si>
+    <t>execute</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>loginlogoutTest</t>
+  </si>
+  <si>
+    <t>newtest</t>
+  </si>
+  <si>
+    <t>To verify login logout functionality</t>
+  </si>
+  <si>
+    <t>To Test</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
   <si>
     <t>testname</t>
   </si>
   <si>
-    <t>testdescription</t>
-  </si>
-  <si>
-    <t>execute</t>
-  </si>
-  <si>
-    <t>priority</t>
-  </si>
-  <si>
-    <t>count</t>
-  </si>
-  <si>
-    <t>newtest</t>
-  </si>
-  <si>
-    <t>to check whether user can successfully login and logout</t>
-  </si>
-  <si>
-    <t>to check execution</t>
-  </si>
-  <si>
-    <t>yes</t>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
   <si>
     <t>no</t>
   </si>
   <si>
-    <t>loginlogoutTest</t>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>QATHOR1005MIG</t>
+  </si>
+  <si>
+    <t>ThorMigration@12345</t>
   </si>
 </sst>
 </file>
@@ -101,8 +117,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -137,7 +155,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -149,7 +167,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -196,23 +214,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -248,23 +249,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -416,39 +400,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB3162B0-60F1-4C12-90DD-CEB9603839DE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -456,11 +440,11 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -471,13 +455,117 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABC0D23-B210-437B-B3BD-0CFD3582C3A9}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rtery failed testcases and IAnnotation Transformer to remove annotations from @Test
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{03E8BCAA-FF3E-473E-86C9-12A12C811D3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{62D2E53B-75EE-41CC-B389-EC69745A46C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15465" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15555" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -474,7 +474,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,7 +545,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Added custom annotation,parallel cross browser code
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{62D2E53B-75EE-41CC-B389-EC69745A46C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3A5E49FD-4273-4D1C-8663-A7D6CA46B4D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="15555" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="20760" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
-    <sheet name="DATA" sheetId="3" r:id="rId2"/>
+    <sheet name="DATA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I14"/>
+  <oleSize ref="A1:M12"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="33">
+  <si>
+    <t>testname</t>
+  </si>
   <si>
     <t>testdescription</t>
   </si>
@@ -39,39 +42,36 @@
     <t>loginlogoutTest</t>
   </si>
   <si>
+    <t>To verify login logout functionality</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>newtest</t>
   </si>
   <si>
-    <t>To verify login logout functionality</t>
-  </si>
-  <si>
     <t>To Test</t>
   </si>
   <si>
     <t>yes</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
-    <t>testname</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
     <t>password</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -82,6 +82,45 @@
   </si>
   <si>
     <t>ThorMigration@12345</t>
+  </si>
+  <si>
+    <t>verifyNewUser</t>
+  </si>
+  <si>
+    <t>To verify creation of new user</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>primaryemail</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Mayur</t>
+  </si>
+  <si>
+    <t>Sapre</t>
+  </si>
+  <si>
+    <t>testautomation0504@gmail.com</t>
+  </si>
+  <si>
+    <t>Add &amp; manage users</t>
   </si>
 </sst>
 </file>
@@ -117,7 +156,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -401,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,54 +456,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
+      <c r="E4" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -470,102 +529,224 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABC0D23-B210-437B-B3BD-0CFD3582C3A9}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{556B7DE6-35DF-42ED-97EB-77FDE3D7E379}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="F2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E6" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="F6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E7" s="5" t="s">
         <v>19</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Docker-update runmode in property file,RUNMODE in enum and handle runmode as remote or local in driver class
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A93A526C-B723-4DE0-8082-F0B466DE0991}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BC5E0414-2D8B-4F6C-A57C-F6372C12F707}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1410" windowWidth="20760" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1800" windowWidth="20910" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
     <sheet name="DATA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I11"/>
+  <oleSize ref="A1:G12"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="39">
   <si>
     <t>testname</t>
   </si>
@@ -81,85 +81,64 @@
     <t>QATHOR1005MIG</t>
   </si>
   <si>
+    <t>verifyNewUser</t>
+  </si>
+  <si>
+    <t>To verify creation of new user</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>primaryemail</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Mayur</t>
+  </si>
+  <si>
+    <t>Sapre</t>
+  </si>
+  <si>
+    <t>testautomation0504@gmail.com</t>
+  </si>
+  <si>
+    <t>Add &amp; manage users</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>Bhoomi</t>
+  </si>
+  <si>
+    <t>Watane</t>
+  </si>
+  <si>
+    <t>gfdcdghd</t>
+  </si>
+  <si>
+    <t>sjdcdfh</t>
+  </si>
+  <si>
+    <t>cfjefewrvjr</t>
+  </si>
+  <si>
     <t>ThorMigration@12345</t>
-  </si>
-  <si>
-    <t>verifyNewUser</t>
-  </si>
-  <si>
-    <t>To verify creation of new user</t>
-  </si>
-  <si>
-    <t>browser</t>
-  </si>
-  <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
-    <t>primaryemail</t>
-  </si>
-  <si>
-    <t>menu</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Mayur</t>
-  </si>
-  <si>
-    <t>Sapre</t>
-  </si>
-  <si>
-    <t>testautomation0504@gmail.com</t>
-  </si>
-  <si>
-    <t>Add &amp; manage users</t>
-  </si>
-  <si>
-    <t>TestCaseId</t>
-  </si>
-  <si>
-    <t>TestCase_001</t>
-  </si>
-  <si>
-    <t>TestCase_002</t>
-  </si>
-  <si>
-    <t>TestCase_003</t>
-  </si>
-  <si>
-    <t>TestCase_004</t>
-  </si>
-  <si>
-    <t>TestCase_005</t>
-  </si>
-  <si>
-    <t>TestCase_006</t>
-  </si>
-  <si>
-    <t>run</t>
-  </si>
-  <si>
-    <t>Bhoomi</t>
-  </si>
-  <si>
-    <t>Watane</t>
-  </si>
-  <si>
-    <t>gfdcdghd</t>
-  </si>
-  <si>
-    <t>sjdcdfh</t>
-  </si>
-  <si>
-    <t>cfjefewrvjr</t>
   </si>
 </sst>
 </file>
@@ -554,10 +533,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
         <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -580,38 +559,37 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="3"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.42578125" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="8" max="8" width="31.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="3" t="s">
         <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
       </c>
       <c r="G1" t="s">
         <v>24</v>
@@ -622,188 +600,170 @@
       <c r="I1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="F2" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="G2" s="4" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>19</v>
+      <c r="E3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>43</v>
+      <c r="E4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>44</v>
+      <c r="F5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>45</v>
+      <c r="F6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
       </c>
+      <c r="C7" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="D7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="E7" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="F7" s="5" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>29</v>
@@ -813,9 +773,6 @@
       </c>
       <c r="I7" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Docker related components and Elastic Search
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BC5E0414-2D8B-4F6C-A57C-F6372C12F707}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2B932CC8-C087-4B01-824F-294B153E2BE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1800" windowWidth="20910" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="1020" windowWidth="20820" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
     <sheet name="DATA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:G12"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
   <si>
     <t>testname</t>
   </si>
@@ -139,6 +139,24 @@
   </si>
   <si>
     <t>ThorMigration@12345</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>79.0.3945.117</t>
+  </si>
+  <si>
+    <t>91.0.4472.77</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>89.0</t>
+  </si>
+  <si>
+    <t>SapreTest</t>
   </si>
 </sst>
 </file>
@@ -471,7 +489,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,9 +540,9 @@
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -545,7 +563,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -556,20 +574,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{556B7DE6-35DF-42ED-97EB-77FDE3D7E379}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="3"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="8" max="8" width="31.42578125" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="9" max="9" width="31.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -583,21 +602,24 @@
         <v>21</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -611,22 +633,25 @@
       <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="H2" s="4" t="s">
         <v>27</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -640,22 +665,25 @@
       <c r="C3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="H3" s="4" t="s">
         <v>27</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -669,22 +697,25 @@
       <c r="C4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="H4" s="4" t="s">
         <v>27</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -698,22 +729,25 @@
       <c r="C5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="H5" s="4" t="s">
         <v>27</v>
       </c>
       <c r="I5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -727,22 +761,25 @@
       <c r="C6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="H6" s="4" t="s">
         <v>27</v>
       </c>
       <c r="I6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -751,27 +788,94 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="J7" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Integration with ELK stack,Reportportal
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2B932CC8-C087-4B01-824F-294B153E2BE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C3E57335-1AFC-4A4D-BCB8-7620EBEECE99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="1020" windowWidth="20820" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="1410" windowWidth="20940" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
     <sheet name="DATA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:I15"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -489,7 +489,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,13 +523,13 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{556B7DE6-35DF-42ED-97EB-77FDE3D7E379}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,7 +692,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>22</v>
@@ -724,7 +724,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>22</v>
@@ -788,7 +788,7 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>22</v>
@@ -852,7 +852,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
Final commit without Selenoid
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C3E57335-1AFC-4A4D-BCB8-7620EBEECE99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7FB1189B-6ED4-40B4-9932-BE3E6A653C0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1410" windowWidth="20940" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="3015" windowWidth="20610" windowHeight="11820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
     <sheet name="DATA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I15"/>
+  <oleSize ref="A1:I14"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="40">
   <si>
     <t>testname</t>
   </si>
@@ -121,21 +121,6 @@
   </si>
   <si>
     <t>run</t>
-  </si>
-  <si>
-    <t>Bhoomi</t>
-  </si>
-  <si>
-    <t>Watane</t>
-  </si>
-  <si>
-    <t>gfdcdghd</t>
-  </si>
-  <si>
-    <t>sjdcdfh</t>
-  </si>
-  <si>
-    <t>cfjefewrvjr</t>
   </si>
   <si>
     <t>ThorMigration@12345</t>
@@ -489,7 +474,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,7 +514,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -545,8 +530,8 @@
       <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
+      <c r="E3" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -557,7 +542,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>9</v>
@@ -576,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{556B7DE6-35DF-42ED-97EB-77FDE3D7E379}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +587,7 @@
         <v>21</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>14</v>
@@ -643,7 +628,7 @@
         <v>17</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>27</v>
@@ -660,7 +645,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>22</v>
@@ -672,10 +657,10 @@
         <v>18</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>27</v>
@@ -704,10 +689,10 @@
         <v>18</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>27</v>
@@ -739,7 +724,7 @@
         <v>17</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>27</v>
@@ -768,10 +753,10 @@
         <v>18</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>27</v>
@@ -794,13 +779,13 @@
         <v>22</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>28</v>
@@ -826,13 +811,13 @@
         <v>22</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>29</v>
@@ -855,19 +840,19 @@
         <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>28</v>

</xml_diff>